<commit_message>
update date time in lux data
</commit_message>
<xml_diff>
--- a/Discharge/Area_ratingcurve.xlsx
+++ b/Discharge/Area_ratingcurve.xlsx
@@ -8,13 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1cba20500feb7d90/Documents/LongTermData_CayambeCoca/Discharge/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{B217CFCC-B1E2-4B36-A214-101AA7618F6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="507" documentId="8_{8ACDB2FF-B211-4D6E-BFC7-A56DE14FFCFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9CBD511D-DDBB-47C4-BE36-34E1A4496FDD}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="350" windowWidth="8720" windowHeight="9730" activeTab="1" xr2:uid="{4E66E23F-A49D-4849-898B-E5DB46569C61}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{4E66E23F-A49D-4849-898B-E5DB46569C61}"/>
   </bookViews>
   <sheets>
     <sheet name="stn01" sheetId="1" r:id="rId1"/>
     <sheet name="stn02" sheetId="2" r:id="rId2"/>
+    <sheet name="stn03" sheetId="3" r:id="rId3"/>
+    <sheet name="stn04" sheetId="4" r:id="rId4"/>
+    <sheet name="stn05" sheetId="5" r:id="rId5"/>
+    <sheet name="stn06" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="17">
   <si>
     <t>Station</t>
   </si>
@@ -60,18 +64,64 @@
   <si>
     <t>stn02</t>
   </si>
+  <si>
+    <t>no time stamp</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>stn03</t>
+  </si>
+  <si>
+    <t>trapazoid method</t>
+  </si>
+  <si>
+    <t>stn04</t>
+  </si>
+  <si>
+    <t>stn05</t>
+  </si>
+  <si>
+    <t>stn06</t>
+  </si>
+  <si>
+    <t>time_used</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -94,9 +144,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -539,7 +596,969 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.40010619310578305"/>
+                  <c:y val="-3.0333977039818973E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                      <a:t>y = 1.1168x + 0.0095</a:t>
+                    </a:r>
+                    <a:br>
+                      <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                    </a:br>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                      <a:t>R² = 0.6446</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" sz="2000"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'stn04'!$J$3:$J$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.005138E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6557189999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0850210000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.7209979999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.2016299999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.4942750000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.3386029999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.1690000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.2481930000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.5401620000000002E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'stn04'!$K$3:$K$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.0450000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.9300000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.1150000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.6300000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.2200000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.1949999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.0924400000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.9999999999999988E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.1499999999999992E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.8599999999999994E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6F2F-4B69-A663-FAF888FB38D3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1396972176"/>
+        <c:axId val="1396970736"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1396972176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1396970736"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1396970736"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1396972176"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.40322681539807526"/>
+                  <c:y val="-7.8926071741032364E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1800" baseline="0"/>
+                      <a:t>y = 0.9563x - 0.0621</a:t>
+                    </a:r>
+                    <a:br>
+                      <a:rPr lang="en-US" sz="1800" baseline="0"/>
+                    </a:br>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1800" baseline="0"/>
+                      <a:t>R² = 0.4135</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" sz="3600"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'stn04'!$J$13:$J$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.1329786</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.13346810000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.4593659999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.12646569999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.13220670000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.1548649</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.18678210000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'stn04'!$K$13:$K$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.7500000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.1949999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.1250000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.6000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.6249999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.11999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.12180000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-23BC-4CD1-9C27-E2592E691E13}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1282469344"/>
+        <c:axId val="1282470304"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1282469344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1282470304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1282470304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1282469344"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1095,6 +2114,1038 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1128,6 +3179,83 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>370417</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>574675</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>54412</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{463757E0-579B-9237-9A0B-68C6171C1D69}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>132292</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>226484</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>407458</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>175684</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E0AB37A-4FCF-D720-242D-AF25BD5C6AAD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1798,10 +3926,1325 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5D94D15-3EB9-4099-97A0-F31D3727D622}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="15.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1">
+        <v>44357.507638888892</v>
+      </c>
+      <c r="C2">
+        <v>1.8200000000000001E-2</v>
+      </c>
+      <c r="D2">
+        <v>2.5905000000000004E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1">
+        <v>44358.440972222219</v>
+      </c>
+      <c r="C3">
+        <v>3.1400000000000004E-2</v>
+      </c>
+      <c r="D3">
+        <v>8.7300000000000016E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1">
+        <v>44361.447222222225</v>
+      </c>
+      <c r="C4">
+        <v>7.1499999999999994E-2</v>
+      </c>
+      <c r="D4">
+        <v>3.3599999999999984E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1">
+        <v>44365.5</v>
+      </c>
+      <c r="C5">
+        <v>8.9499999999999996E-3</v>
+      </c>
+      <c r="D5">
+        <v>1.5699999999999998E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1">
+        <v>44372.498611111114</v>
+      </c>
+      <c r="C6">
+        <v>3.9699999999999999E-2</v>
+      </c>
+      <c r="D6">
+        <v>1.2390000000000003E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1">
+        <v>44375.5</v>
+      </c>
+      <c r="C7">
+        <v>6.0250000000000005E-2</v>
+      </c>
+      <c r="D7">
+        <v>6.1150000000000006E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>44382.447916666664</v>
+      </c>
+      <c r="C8">
+        <v>0.104</v>
+      </c>
+      <c r="D8">
+        <v>1.2370000000000001E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1">
+        <v>44386.456944444442</v>
+      </c>
+      <c r="C9">
+        <v>5.5244999999999995E-2</v>
+      </c>
+      <c r="D9">
+        <v>1.5533370000000005E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="1">
+        <v>44389.590277777781</v>
+      </c>
+      <c r="C10">
+        <v>2.5050000000000003E-2</v>
+      </c>
+      <c r="D10">
+        <v>1.362E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="1">
+        <v>44390.59375</v>
+      </c>
+      <c r="C11">
+        <v>8.7749999999999995E-2</v>
+      </c>
+      <c r="D11">
+        <v>1.9664999999999998E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="1">
+        <v>44391.419444444444</v>
+      </c>
+      <c r="C12">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="D12">
+        <v>2.2250000000000002E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="1">
+        <v>44393.5</v>
+      </c>
+      <c r="C13">
+        <v>7.6E-3</v>
+      </c>
+      <c r="D13">
+        <v>1.9400000000000001E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="1">
+        <v>44397.547222222223</v>
+      </c>
+      <c r="C14">
+        <v>7.9499999999999987E-2</v>
+      </c>
+      <c r="D14">
+        <v>5.8285000000000003E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="1">
+        <v>44400.46875</v>
+      </c>
+      <c r="C15">
+        <v>0.13449999999999998</v>
+      </c>
+      <c r="D15">
+        <v>7.0059999999999997E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="1">
+        <v>44403.583333333336</v>
+      </c>
+      <c r="C16">
+        <v>0.13879999999999998</v>
+      </c>
+      <c r="D16">
+        <v>1.3055999999999996E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="1">
+        <v>44404.5625</v>
+      </c>
+      <c r="C17">
+        <v>8.5699999999999998E-2</v>
+      </c>
+      <c r="D17">
+        <v>1.1249E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="1">
+        <v>44489.5</v>
+      </c>
+      <c r="C18">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="D18">
+        <v>7.3900000000000007E-4</v>
+      </c>
+      <c r="F18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="1">
+        <v>44714.520833333336</v>
+      </c>
+      <c r="C19">
+        <v>1.4999999999999998E-2</v>
+      </c>
+      <c r="D19">
+        <v>4.1500000000000009E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="1">
+        <v>44719.465277777781</v>
+      </c>
+      <c r="C20">
+        <v>0.12375000000000001</v>
+      </c>
+      <c r="D20">
+        <v>6.0600000000000011E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="1">
+        <v>44742.524305555555</v>
+      </c>
+      <c r="C21">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="D21">
+        <v>1.213E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="1">
+        <v>44764.388194444444</v>
+      </c>
+      <c r="C22">
+        <v>0.11225000000000002</v>
+      </c>
+      <c r="D22">
+        <v>2.6637500000000008E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="1">
+        <v>44769.409722222219</v>
+      </c>
+      <c r="C23">
+        <v>6.9300000000000014E-2</v>
+      </c>
+      <c r="D23">
+        <v>7.3080000000000011E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE05374E-456A-4C73-BBA7-E0082822A06A}">
+  <dimension ref="A1:F25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="15.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1">
+        <v>44356.512499999997</v>
+      </c>
+      <c r="C2">
+        <v>1.1100000000000002E-2</v>
+      </c>
+      <c r="D2">
+        <v>3.4809999999999997E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1">
+        <v>44357.590277777781</v>
+      </c>
+      <c r="C3">
+        <v>8.6999999999999994E-3</v>
+      </c>
+      <c r="D3">
+        <v>2.2440000000000003E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1">
+        <v>44358.46597222222</v>
+      </c>
+      <c r="C4">
+        <v>6.2999999999999992E-3</v>
+      </c>
+      <c r="D4">
+        <v>1.6169999999999999E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1">
+        <v>44361.469444444447</v>
+      </c>
+      <c r="C5">
+        <v>4.2000000000000006E-3</v>
+      </c>
+      <c r="D5">
+        <v>5.1240000000000009E-3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1">
+        <v>44365.541666666664</v>
+      </c>
+      <c r="C6">
+        <v>1.44E-2</v>
+      </c>
+      <c r="D6">
+        <v>3.0559999999999997E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1">
+        <v>44372.520833333336</v>
+      </c>
+      <c r="C7">
+        <v>2.2700000000000001E-2</v>
+      </c>
+      <c r="D7">
+        <v>7.064E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="1">
+        <v>44375.534722222219</v>
+      </c>
+      <c r="C8">
+        <v>2.0299999999999999E-2</v>
+      </c>
+      <c r="D8">
+        <v>5.1710000000000002E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="1">
+        <v>44382.458333333336</v>
+      </c>
+      <c r="C9">
+        <v>4.0500000000000001E-2</v>
+      </c>
+      <c r="D9">
+        <v>1.2959999999999999E-2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1">
+        <v>44386.489583333336</v>
+      </c>
+      <c r="C10">
+        <v>4.7929799999999995E-2</v>
+      </c>
+      <c r="D10">
+        <v>8.055101999999998E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>44389.607638888891</v>
+      </c>
+      <c r="C11">
+        <v>6.7299999999999999E-2</v>
+      </c>
+      <c r="D11">
+        <v>2.2453999999999998E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1">
+        <v>44390.607638888891</v>
+      </c>
+      <c r="C12">
+        <v>4.9550000000000004E-2</v>
+      </c>
+      <c r="D12">
+        <v>1.8588E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="1">
+        <v>44391.568055555559</v>
+      </c>
+      <c r="C13">
+        <v>4.7500000000000001E-2</v>
+      </c>
+      <c r="D13">
+        <v>8.0300000000000024E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="1">
+        <v>44393.527777777781</v>
+      </c>
+      <c r="C14">
+        <v>1.1499999999999993E-2</v>
+      </c>
+      <c r="D14">
+        <v>4.4509999999999975E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="1">
+        <v>44396.482638888891</v>
+      </c>
+      <c r="C15">
+        <v>0.222</v>
+      </c>
+      <c r="D15">
+        <v>0.23874000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="1">
+        <v>44397.416666666664</v>
+      </c>
+      <c r="C16">
+        <v>8.0999999999999989E-2</v>
+      </c>
+      <c r="D16">
+        <v>9.1047500000000003E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="1">
+        <v>44400.5</v>
+      </c>
+      <c r="C17">
+        <v>6.0350000000000001E-2</v>
+      </c>
+      <c r="D17">
+        <v>7.2412500000000019E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="1">
+        <v>44403.635416666664</v>
+      </c>
+      <c r="C18">
+        <v>3.1449999999999999E-2</v>
+      </c>
+      <c r="D18">
+        <v>2.4760500000000001E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="1">
+        <v>44404.458333333336</v>
+      </c>
+      <c r="C19">
+        <v>2.9300000000000007E-2</v>
+      </c>
+      <c r="D19">
+        <v>1.4876000000000004E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="1">
+        <v>44489.5</v>
+      </c>
+      <c r="C20">
+        <v>2.5999999999999995E-2</v>
+      </c>
+      <c r="D20">
+        <v>1.4179999999999996E-3</v>
+      </c>
+      <c r="F20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="1">
+        <v>44714.590277777781</v>
+      </c>
+      <c r="C21">
+        <v>3.4500000000000003E-2</v>
+      </c>
+      <c r="D21">
+        <v>3.5700000000000003E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="1">
+        <v>44719.480555555558</v>
+      </c>
+      <c r="C22">
+        <v>1.8499999999999996E-2</v>
+      </c>
+      <c r="D22">
+        <v>3.1700000000000001E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="1">
+        <v>44741.53125</v>
+      </c>
+      <c r="C23">
+        <v>5.2749999999999998E-2</v>
+      </c>
+      <c r="D23">
+        <v>1.3154999999999998E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="1">
+        <v>44764.482638888891</v>
+      </c>
+      <c r="C24">
+        <v>0.14699999999999994</v>
+      </c>
+      <c r="D24">
+        <v>1.933E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="1">
+        <v>44769.432638888888</v>
+      </c>
+      <c r="C25">
+        <v>7.3800000000000018E-2</v>
+      </c>
+      <c r="D25">
+        <v>2.3090000000000003E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4196674-093B-4988-AB0C-54D57CD03A2F}">
+  <dimension ref="A1:K19"/>
+  <sheetViews>
+    <sheetView zoomScale="60" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="8.7265625" style="2"/>
+    <col min="2" max="2" width="21.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="8.90625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="8.7265625" style="2"/>
+    <col min="9" max="9" width="21.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="8.90625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.7265625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="3">
+        <v>44357.5625</v>
+      </c>
+      <c r="C2" s="2">
+        <v>2.2050000000000004E-2</v>
+      </c>
+      <c r="D2" s="2">
+        <v>3.5975000000000013E-3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="3">
+        <v>44357.5625</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="2">
+        <v>2.2050000000000004E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="3">
+        <v>44358.474999999999</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1.0450000000000001E-2</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1.6005000000000008E-3</v>
+      </c>
+      <c r="E3" s="4">
+        <v>1.005138E-2</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0.46875</v>
+      </c>
+      <c r="I3" s="3">
+        <v>44358.474999999999</v>
+      </c>
+      <c r="J3" s="4">
+        <v>1.005138E-2</v>
+      </c>
+      <c r="K3" s="2">
+        <v>1.0450000000000001E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="3">
+        <v>44361.479166666664</v>
+      </c>
+      <c r="C4" s="2">
+        <v>2.9300000000000003E-2</v>
+      </c>
+      <c r="D4" s="2">
+        <v>3.6880000000000003E-3</v>
+      </c>
+      <c r="E4" s="6">
+        <v>1.6557189999999999E-2</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="I4" s="3">
+        <v>44361.479166666664</v>
+      </c>
+      <c r="J4" s="6">
+        <v>1.6557189999999999E-2</v>
+      </c>
+      <c r="K4" s="2">
+        <v>2.9300000000000003E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="3">
+        <v>44365.581250000003</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2.1150000000000002E-2</v>
+      </c>
+      <c r="D5" s="2">
+        <v>4.889000000000001E-3</v>
+      </c>
+      <c r="E5" s="6">
+        <v>2.0850210000000001E-2</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="I5" s="3">
+        <v>44365.581250000003</v>
+      </c>
+      <c r="J5" s="6">
+        <v>2.0850210000000001E-2</v>
+      </c>
+      <c r="K5" s="2">
+        <v>2.1150000000000002E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="3">
+        <v>44372.541666666664</v>
+      </c>
+      <c r="C6" s="2">
+        <v>5.6300000000000003E-2</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1.1621000000000005E-2</v>
+      </c>
+      <c r="E6" s="6">
+        <v>4.7209979999999999E-2</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="I6" s="3">
+        <v>44372.541666666664</v>
+      </c>
+      <c r="J6" s="6">
+        <v>4.7209979999999999E-2</v>
+      </c>
+      <c r="K6" s="2">
+        <v>5.6300000000000003E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="3">
+        <v>44375.551388888889</v>
+      </c>
+      <c r="C7" s="2">
+        <v>3.2200000000000006E-2</v>
+      </c>
+      <c r="D7" s="2">
+        <v>7.1710000000000003E-3</v>
+      </c>
+      <c r="E7" s="6">
+        <v>6.2016299999999996E-3</v>
+      </c>
+      <c r="F7" s="5">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="I7" s="3">
+        <v>44375.551388888889</v>
+      </c>
+      <c r="J7" s="6">
+        <v>6.2016299999999996E-3</v>
+      </c>
+      <c r="K7" s="2">
+        <v>3.2200000000000006E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="3">
+        <v>44382.472222222219</v>
+      </c>
+      <c r="C8" s="2">
+        <v>2.1949999999999997E-2</v>
+      </c>
+      <c r="D8" s="2">
+        <v>7.1900000000000002E-3</v>
+      </c>
+      <c r="E8" s="6">
+        <v>3.4942750000000002E-2</v>
+      </c>
+      <c r="F8" s="5">
+        <v>0.46875</v>
+      </c>
+      <c r="I8" s="3">
+        <v>44382.472222222219</v>
+      </c>
+      <c r="J8" s="6">
+        <v>3.4942750000000002E-2</v>
+      </c>
+      <c r="K8" s="2">
+        <v>2.1949999999999997E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="3">
+        <v>44386.504166666666</v>
+      </c>
+      <c r="C9" s="2">
+        <v>8.0924400000000007E-2</v>
+      </c>
+      <c r="D9" s="2">
+        <v>9.1592400000000008E-3</v>
+      </c>
+      <c r="E9" s="6">
+        <v>4.3386029999999999E-2</v>
+      </c>
+      <c r="F9" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="I9" s="3">
+        <v>44386.504166666666</v>
+      </c>
+      <c r="J9" s="6">
+        <v>4.3386029999999999E-2</v>
+      </c>
+      <c r="K9" s="2">
+        <v>8.0924400000000007E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="3">
+        <v>44389.625</v>
+      </c>
+      <c r="C10" s="2">
+        <v>7.9999999999999988E-2</v>
+      </c>
+      <c r="D10" s="2">
+        <v>2.734E-2</v>
+      </c>
+      <c r="E10" s="6">
+        <v>6.1690000000000002E-2</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0.625</v>
+      </c>
+      <c r="I10" s="3">
+        <v>44389.625</v>
+      </c>
+      <c r="J10" s="6">
+        <v>6.1690000000000002E-2</v>
+      </c>
+      <c r="K10" s="2">
+        <v>7.9999999999999988E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="3">
+        <v>44390.614583333336</v>
+      </c>
+      <c r="C11" s="2">
+        <v>6.1499999999999992E-2</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1.6489999999999998E-2</v>
+      </c>
+      <c r="E11" s="6">
+        <v>5.2481930000000003E-2</v>
+      </c>
+      <c r="F11" s="5">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="I11" s="3">
+        <v>44390.614583333336</v>
+      </c>
+      <c r="J11" s="6">
+        <v>5.2481930000000003E-2</v>
+      </c>
+      <c r="K11" s="2">
+        <v>6.1499999999999992E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="3">
+        <v>44391.584722222222</v>
+      </c>
+      <c r="C12" s="2">
+        <v>6.8599999999999994E-2</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1.0310000000000003E-2</v>
+      </c>
+      <c r="E12" s="6">
+        <v>3.5401620000000002E-2</v>
+      </c>
+      <c r="F12" s="5">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="I12" s="3">
+        <v>44391.584722222222</v>
+      </c>
+      <c r="J12" s="6">
+        <v>3.5401620000000002E-2</v>
+      </c>
+      <c r="K12" s="2">
+        <v>6.8599999999999994E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3">
+        <v>44403.541666666664</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1.7500000000000002E-2</v>
+      </c>
+      <c r="D13" s="2">
+        <v>3.8230000000000004E-3</v>
+      </c>
+      <c r="E13" s="6">
+        <v>0.1329786</v>
+      </c>
+      <c r="F13" s="5">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="I13" s="3">
+        <v>44403.541666666664</v>
+      </c>
+      <c r="J13" s="6">
+        <v>0.1329786</v>
+      </c>
+      <c r="K13" s="2">
+        <v>1.7500000000000002E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="3">
+        <v>44404.427083333336</v>
+      </c>
+      <c r="C14" s="2">
+        <v>6.1949999999999998E-2</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1.4605999999999999E-2</v>
+      </c>
+      <c r="E14" s="6">
+        <v>0.13346810000000001</v>
+      </c>
+      <c r="F14" s="5">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="I14" s="3">
+        <v>44404.427083333336</v>
+      </c>
+      <c r="J14" s="6">
+        <v>0.13346810000000001</v>
+      </c>
+      <c r="K14" s="2">
+        <v>6.1949999999999998E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="3">
+        <v>44489.5</v>
+      </c>
+      <c r="C15" s="2">
+        <v>5.1250000000000004E-2</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1.7767500000000003E-3</v>
+      </c>
+      <c r="E15" s="6">
+        <v>9.4593659999999996E-2</v>
+      </c>
+      <c r="F15" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I15" s="3">
+        <v>44489.5</v>
+      </c>
+      <c r="J15" s="6">
+        <v>9.4593659999999996E-2</v>
+      </c>
+      <c r="K15" s="2">
+        <v>5.1250000000000004E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="3">
+        <v>44714.571527777778</v>
+      </c>
+      <c r="C16" s="2">
+        <v>8.6000000000000007E-2</v>
+      </c>
+      <c r="D16" s="2">
+        <v>5.3999999999999994E-3</v>
+      </c>
+      <c r="E16" s="6">
+        <v>0.12646569999999999</v>
+      </c>
+      <c r="F16" s="5">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="I16" s="3">
+        <v>44714.571527777778</v>
+      </c>
+      <c r="J16" s="6">
+        <v>0.12646569999999999</v>
+      </c>
+      <c r="K16" s="2">
+        <v>8.6000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="3">
+        <v>44719.498611111114</v>
+      </c>
+      <c r="C17" s="2">
+        <v>2.6249999999999999E-2</v>
+      </c>
+      <c r="D17" s="2">
+        <v>2.8125000000000003E-3</v>
+      </c>
+      <c r="E17" s="6">
+        <v>0.13220670000000001</v>
+      </c>
+      <c r="F17" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="I17" s="3">
+        <v>44719.498611111114</v>
+      </c>
+      <c r="J17" s="6">
+        <v>0.13220670000000001</v>
+      </c>
+      <c r="K17" s="2">
+        <v>2.6249999999999999E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="3">
+        <v>44764.45416666667</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.11999999999999998</v>
+      </c>
+      <c r="D18" s="2">
+        <v>2.8740000000000005E-2</v>
+      </c>
+      <c r="E18" s="6">
+        <v>0.1548649</v>
+      </c>
+      <c r="F18" s="5">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="I18" s="3">
+        <v>44764.45416666667</v>
+      </c>
+      <c r="J18" s="6">
+        <v>0.1548649</v>
+      </c>
+      <c r="K18" s="2">
+        <v>0.11999999999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="3">
+        <v>44769.519444444442</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.12180000000000002</v>
+      </c>
+      <c r="D19" s="2">
+        <v>3.1280000000000002E-2</v>
+      </c>
+      <c r="E19" s="6">
+        <v>0.18678210000000001</v>
+      </c>
+      <c r="F19" s="5">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="I19" s="3">
+        <v>44769.519444444442</v>
+      </c>
+      <c r="J19" s="6">
+        <v>0.18678210000000001</v>
+      </c>
+      <c r="K19" s="2">
+        <v>0.12180000000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61EEAE6F-43D7-445F-A93A-9D3A3E280C0B}">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1809,7 +5252,7 @@
     <col min="2" max="2" width="14.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1825,187 +5268,283 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1">
-        <v>44357.507638888892</v>
+        <v>44358.533333333333</v>
       </c>
       <c r="C2">
-        <v>1.8200000000000001E-2</v>
+        <v>0.21800000000000003</v>
       </c>
       <c r="D2">
-        <v>2.5905000000000004E-3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
+        <v>4.7080000000000011E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B3" s="1">
-        <v>44358.440972222219</v>
+        <v>44386.673611111109</v>
       </c>
       <c r="C3">
-        <v>3.1400000000000004E-2</v>
+        <v>0.53349999999999997</v>
       </c>
       <c r="D3">
-        <v>8.7300000000000016E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
+        <v>0.16736999999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B4" s="1">
-        <v>44361.447222222225</v>
+        <v>44391.609027777777</v>
       </c>
       <c r="C4">
-        <v>7.1499999999999994E-2</v>
+        <v>0.255</v>
       </c>
       <c r="D4">
-        <v>3.3599999999999984E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
+        <v>5.0860000000000009E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B5" s="1">
-        <v>44365.5</v>
+        <v>44393.588194444441</v>
       </c>
       <c r="C5">
-        <v>8.9499999999999996E-3</v>
+        <v>0.23099999999999987</v>
       </c>
       <c r="D5">
-        <v>1.5699999999999998E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
+        <v>6.4550000000000066E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B6" s="1">
-        <v>44372.498611111114</v>
+        <v>44398.45</v>
       </c>
       <c r="C6">
-        <v>3.9699999999999999E-2</v>
+        <v>0.56299999999999994</v>
       </c>
       <c r="D6">
-        <v>1.2390000000000003E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
+        <v>0.21695999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B7" s="1">
-        <v>44375.5</v>
+        <v>44400.413194444445</v>
       </c>
       <c r="C7">
-        <v>6.0250000000000005E-2</v>
+        <v>0.74800000000000011</v>
       </c>
       <c r="D7">
-        <v>6.1150000000000006E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
+        <v>0.78109999999999979</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B8" s="1">
-        <v>44382.447916666664</v>
+        <v>44403.614583333336</v>
       </c>
       <c r="C8">
-        <v>0.104</v>
+        <v>0.50600000000000001</v>
       </c>
       <c r="D8">
-        <v>1.2370000000000001E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
+        <v>0.13865999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B9" s="1">
-        <v>44386.456944444442</v>
+        <v>44405.5625</v>
       </c>
       <c r="C9">
-        <v>5.5244999999999995E-2</v>
+        <v>0.37180000000000002</v>
       </c>
       <c r="D9">
-        <v>1.5533370000000005E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
+        <v>8.1770999999999996E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B10" s="1">
-        <v>44389.590277777781</v>
+        <v>44740.551388888889</v>
       </c>
       <c r="C10">
-        <v>2.5050000000000003E-2</v>
+        <v>0.78949999999999998</v>
       </c>
       <c r="D10">
-        <v>1.362E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>7</v>
-      </c>
+        <v>0.10291500000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B11" s="1">
-        <v>44390.59375</v>
+        <v>44768.436111111114</v>
       </c>
       <c r="C11">
-        <v>8.7749999999999995E-2</v>
+        <v>0.70899999999999985</v>
       </c>
       <c r="D11">
-        <v>1.9664999999999998E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>7</v>
-      </c>
+        <v>6.018999999999998E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68A8C2A8-E3AC-4AF6-B19A-B44E59672203}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="14.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1">
+        <v>44358.51666666667</v>
+      </c>
+      <c r="C2">
+        <v>5.5249999999999994E-2</v>
+      </c>
+      <c r="D2">
+        <v>5.5525000000000005E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B3" s="1">
+        <v>44375.430555555555</v>
+      </c>
+      <c r="C3">
+        <v>0.38399999999999995</v>
+      </c>
+      <c r="D3">
+        <v>7.3030000000000012E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B4" s="1">
+        <v>44768.381249999999</v>
+      </c>
+      <c r="C4">
+        <v>0.51475000000000004</v>
+      </c>
+      <c r="D4">
+        <v>0.12222250000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B5" s="1">
+        <v>44740.544444444444</v>
+      </c>
+      <c r="C5">
+        <v>0.45600000000000007</v>
+      </c>
+      <c r="D5">
+        <v>0.12096000000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B6" s="1">
+        <v>44405.572916666664</v>
+      </c>
+      <c r="C6">
+        <v>0.31204999999999999</v>
+      </c>
+      <c r="D6">
+        <v>0.11604049999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B7" s="1">
+        <v>44403.604166666664</v>
+      </c>
+      <c r="C7">
+        <v>0.53374999999999984</v>
+      </c>
+      <c r="D7">
+        <v>0.15804499999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B8" s="1">
+        <v>44400.40625</v>
+      </c>
+      <c r="C8">
+        <v>0.87359999999999993</v>
+      </c>
+      <c r="D8">
+        <v>0.48200800000000005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B9" s="1">
+        <v>44398.427083333336</v>
+      </c>
+      <c r="C9">
+        <v>0.29420000000000002</v>
+      </c>
+      <c r="D9">
+        <v>0.24913800000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B10" s="1">
+        <v>44393.597222222219</v>
+      </c>
+      <c r="C10">
+        <v>0.15825000000000003</v>
+      </c>
+      <c r="D10">
+        <v>7.9015000000000002E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B11" s="1">
+        <v>44391.604861111111</v>
+      </c>
+      <c r="C11">
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="D11">
+        <v>5.9410000000000004E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B12" s="1">
-        <v>44391.419444444444</v>
+        <v>44386.659722222219</v>
       </c>
       <c r="C12">
-        <v>3.5000000000000003E-2</v>
+        <v>0.34199999999999997</v>
       </c>
       <c r="D12">
-        <v>2.2250000000000002E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="1">
-        <v>44393.5</v>
-      </c>
-      <c r="C13">
-        <v>7.6E-3</v>
-      </c>
-      <c r="D13">
-        <v>1.9400000000000001E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="1">
-        <v>44397.547222222223</v>
-      </c>
-      <c r="C14">
-        <v>7.9499999999999987E-2</v>
-      </c>
-      <c r="D14">
-        <v>5.8285000000000003E-2</v>
+        <v>0.13822000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>